<commit_message>
added new layers also improvements for road and kadastra layers
</commit_message>
<xml_diff>
--- a/src/Layers/HH_layers.xlsx
+++ b/src/Layers/HH_layers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VRI\Projekti\HumanHabitat\Human Habitat 2\HH tool\Layers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6C69A5-219C-4047-9365-C711F050FEBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E838D313-3A2B-47BB-A1A8-C10C9588DBA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{13951075-93B7-4C45-B806-104DD06C9588}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{13951075-93B7-4C45-B806-104DD06C9588}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>10101.tif</t>
   </si>
@@ -45,292 +45,220 @@
     <t>10102.tif</t>
   </si>
   <si>
-    <t xml:space="preserve">Datu slānis reprezentē tuvumu līdz Cēsu centram brauciena distances izteiksmē ar 10 km soli, kur 100 punkti atbilst attālumam 0...10 k, 90 punkti attālumam 10…20 km, bet 10 punkti attālumam &gt;90 km. Vērtību aprēķiņāšanai izmantots OpenRoutingService algoritms. </t>
-  </si>
-  <si>
     <t>10103.tif</t>
   </si>
   <si>
     <t xml:space="preserve">Datu slānis reprezentē tuvumu līdz ciematiem jeb sekundāriem centriem Cēsu novadā brauciena laika izteiksmē ar 10 min. soli, kur 100 punkti atbilst attālumam 0...10 min., 90 punkti attālumam 10…20 min., bet 10 punkti attālumam &gt;90 min. Vērtību aprēķiņāšanai izmantots OpenRoutingService algoritms. </t>
   </si>
   <si>
-    <t>10104.tif</t>
-  </si>
-  <si>
-    <t>Tuvums līdz novada centram (laiks)</t>
-  </si>
-  <si>
-    <t>Tuvums līdz sekundāram centram (laiks)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Datu slānis reprezentē tuvumu līdz novadu centriem brauciena laika izteiksmē ar 10 min. soli, kur 100 punkti atbilst attālumam 0...10 min., 90 punkti attālumam 10…20 min., bet 10 punkti attālumam &gt;90 min. Vērtību aprēķiņāšanai izmantots OpenRoutingService algoritms. </t>
   </si>
   <si>
-    <t>Tuvums līdz novada centram (distance)</t>
-  </si>
-  <si>
-    <t>Tuvums līdz Cēsīm (laiks)</t>
-  </si>
-  <si>
-    <t>Tuvums līdz Cēsīm (distance)</t>
-  </si>
-  <si>
-    <t>10105.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Datu slānis reprezentē tuvumu līdz novadu centriem brauciena distances izteiksmē ar 10 km soli, kur 100 punkti atbilst attālumam 0...10 k, 90 punkti attālumam 10…20 km, bet 10 punkti attālumam &gt;90 km. Vērtību aprēķiņāšanai izmantots OpenRoutingService algoritms. </t>
-  </si>
-  <si>
     <t>10301.tif</t>
   </si>
   <si>
-    <t>10302.tif</t>
-  </si>
-  <si>
-    <t>Ūdenstilpes (&gt;0,1 ha)</t>
-  </si>
-  <si>
-    <t>Ūdenstilpes (&gt;1 ha)</t>
-  </si>
-  <si>
-    <t>Ūdenstilpes (&gt;50 ha)</t>
-  </si>
-  <si>
-    <t>10303.tif</t>
-  </si>
-  <si>
-    <t>Meži (&gt;0,1 ha)</t>
+    <t>Datu slānis reprezentē ūdenstilpes (&gt;1 ha) tuvumu, kur 100 punkti atbilst atrašānās ūdenstipē vai tās krastā, 0 punkti &gt;1km attālumā. Ūdenstilpju slānis iegūts kombinējot Zemes seguma klasifikācijas rezultātu ar Open StreetMap datiem.</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē meža (&gt;1 ha) tuvumu, kur 100 punkti atbilst atrašānās mežā vai tā malā, 0 punkti &gt;1km attālumā. Mežu slānis iegūts no Zemes seguma klasifikācijas rezultāta.</t>
+  </si>
+  <si>
+    <t>10501.tif</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē zālāju (&gt;0,1 ha) tuvumu, kur 100 punkti atbilst atrašānās zālājā vai tā malā, 0 punkti &gt;1km attālumā. Zālāju slānis iegūts no Zemes seguma klasifikācijas rezultāta, kombinējot ar Lauku atbalsta dienesta datiem.</t>
+  </si>
+  <si>
+    <t>10502.tif</t>
+  </si>
+  <si>
+    <t>Zālāji (bioloģiski vērtīgie)</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē bioloģiski vērtīgo zālāju tuvumu, kur 100 punkti atbilst atrašānās zālājā vai tā malā, 0 punkti &gt;1km attālumā. Bioloģiski vērtīgo zālāju slānis iegūts no Lauku atbalsta dienesta datiem.</t>
+  </si>
+  <si>
+    <t>Lauksaimniecība (bioloģiskā)</t>
+  </si>
+  <si>
+    <t>Lauksaimniecība (konvencionālā)</t>
+  </si>
+  <si>
+    <t>10601.tif</t>
+  </si>
+  <si>
+    <t>10602.tif</t>
+  </si>
+  <si>
+    <t>10603.tif</t>
+  </si>
+  <si>
+    <t>10803.tif</t>
+  </si>
+  <si>
+    <t>Ēkas</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē ēku tuvumu, kur 100 punkti atbilst atrašānās ēkā vai pie tās, 0 punkti &gt;1km attālumā. Ēku slānis iegūts no OpenStreetMap datiem.</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē konvencionāli apsaimniekoto lauksaimniecības zemju tuvumu, kur 100 punkti atbilst atrašānās laukā vai tā malā, 0 punkti &gt;1km attālumā. Lauksaimniecības zemju slānis iegūts no Zemes seguma klasifikācijas rezultāta, kombinējot ar Lauku atbalsta dienesta datiem.</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē bioloģiski apsaimniekoto lauksaimniecības zemju tuvumu, kur 100 punkti atbilst atrašānās laukā vai tā malā, 0 punkti &gt;1km attālumā. Lauksaimniecības zemju slānis iegūts no Zemes seguma klasifikācijas rezultāta, kombinējot ar Lauku atbalsta dienesta datiem.</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē lauksaimniecības zemju (&gt;0,1 ha) tuvumu, kur 100 punkti atbilst atrašānās laukā vai tā malā, 0 punkti &gt;1km attālumā. Lauksaimniecības zemju slānis iegūts no Zemes seguma klasifikācijas rezultāta, kombinējot ar Lauku atbalsta dienesta datiem.</t>
+  </si>
+  <si>
+    <t>Industriāli objekti</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē industriālu objektu tuvumu, kur 100 punkti atbilst atrašānās objektā vai pie tā, 0 punkti &gt;1km attālumā. Industriālo objektu slānis iegūts no OpenStreetMap datiem.</t>
+  </si>
+  <si>
+    <t>10901.tif</t>
+  </si>
+  <si>
+    <t>10902.tif</t>
+  </si>
+  <si>
+    <t>Ceļi (visi)</t>
+  </si>
+  <si>
+    <t>Ceļi (galvenie)</t>
+  </si>
+  <si>
+    <t>Dzelzceļš</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē ar auto izbraucamo ceļu tuvumu, kur 100 punkti atbilst atrašānās uz ceļa vai pie tā, 0 punkti &gt;1km attālumā. Ceļu slānis iegūts no OpenStreetMap datiem.</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē galveno ceļu tuvumu, kur 100 punkti atbilst atrašānās uz ceļa vai pie tā, 0 punkti &gt;1km attālumā. Ceļu slānis iegūts no OpenStreetMap datiem.</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē dzelzceļa tuvumu, kur 100 punkti atbilst atrašānās uz dzelzceļa vai pie tā, 0 punkti &gt;1km attālumā. Dzelzceļa slānis iegūts no OpenStreetMap datiem.</t>
+  </si>
+  <si>
+    <t>Tūrisma objekti</t>
+  </si>
+  <si>
+    <t>Kapsētas</t>
+  </si>
+  <si>
+    <t>Militārie objekti</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē tūrisma objektu tuvumu, kur 100 punkti atbilst atrašānās tūrisma objektā, 0 punkti &gt;1km attālumā. Tūrisma objektu slānis iegūts no OpenStreetMap datiem.</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē militāro objektu tuvumu, kur 100 punkti atbilst atrašānās objektā vai pie tā, 0 punkti &gt;1km attālumā. Militāro objektu slānis iegūts no OpenStreetMap datiem.</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē kapsētu tuvumu, kur 100 punkti atbilst atrašānās kapsētā vai pie tās, 0 punkti &gt;1km attālumā. Kapsētu slānis iegūts no OpenStreetMap datiem.</t>
+  </si>
+  <si>
+    <t>11106.tif</t>
+  </si>
+  <si>
+    <t>11108.tif</t>
+  </si>
+  <si>
+    <t>11109.tif</t>
+  </si>
+  <si>
+    <t>Zaļums (pastāvīgs)</t>
+  </si>
+  <si>
+    <t>Zaļuma pieaugums</t>
+  </si>
+  <si>
+    <t>Zaļuma samazinājums</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē ainavas procentuālo segumu ar veģetāciju, kur 100 punkti atbilst 100% veģetācijas segumam 300 m diametrā, bet 0 punkti - 0%. Pastāvīgā zaļuma novērtējumam izmantoti Sentinel-2 satelītdati 2016.-2019. gadam, NDVI slieksnis 0,5.</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē ainavas procentuālo īpatsvaru ar novērotu zaļuma pieaugumu 2016.-2019. gadā, kur 100 punkti atbilst 100% zaļuma pieaugumam 300 m diametrā, bet 0 punkti - 0%. Zaļuma pieauguma novērtējumam izmantoti Sentinel-2 satelītdati 2016.-2019. gadam, NDVI slieksnis 0,5, skatīta tendence.</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē ainavas procentuālo īpatsvaru ar novērotu zaļuma samazinājumu 2016.-2019. gadā, kur 100 punkti atbilst 100% zaļuma samazinājumam 300 m diametrā, bet 0 punkti - 0%. Zaļuma samazinājuma novērtējumam izmantoti Sentinel-2 satelītdati 2016.-2019. gadam, NDVI slieksnis 0,5, skatīta tendence.</t>
+  </si>
+  <si>
+    <t>Ainavas atvērtums</t>
+  </si>
+  <si>
+    <t>Lokālie pauguri</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē ainavas atvērtumu 300 m radiusā, skatoties no 1,8 m augstuma, kur 100 punkti atbilst pilnīgi atvērtai jeb pārskatāmai ainavai, bet 0 punkti - slēgtai. Datu slāņa izveidei izmantots digitālais virsmas un reljefa modelis.</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē paugurus lokālā reljefā, kur par referenci ņemts vidējais reljefs 300 m radiusā. 100 punkti atbilst pauguram, kas par 10 un vairām metriem paceļas virs vidējā ainavas augstuma, 90 punkti - 9 m, bet 0 punkti vidējam lokālā reljefa augstumam vai zemākam.</t>
+  </si>
+  <si>
+    <t>Datu slānis reprezentē ieplakas lokālā reljefā, kur par referenci ņemts vidējais reljefs 300 m radiusā. 100 punkti atbilst ieplakai, kas par 10 un vairām metriem iegrimst zem vidējā ainavas augstuma, 90 punkti - 9 m, bet 0 punkti vidējam lokālā reljefa augstumam vai augstākam.</t>
+  </si>
+  <si>
+    <t>Lokālās ieplakas</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Layer</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Ūdenstilpes</t>
+  </si>
+  <si>
+    <t>Meži</t>
+  </si>
+  <si>
+    <t>Zālāji</t>
   </si>
   <si>
     <t>10401.tif</t>
   </si>
   <si>
-    <t>Meži (&gt;1 ha)</t>
-  </si>
-  <si>
-    <t>10402.tif</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē ūdenstilpes (&gt;0,1 ha) tuvumu, kur 100 punkti atbilst atrašānās ūdenstipē vai tās krastā, 0 punkti &gt;1km attālumā. Ūdenstilpju slānis iegūts kombinējot Zemes seguma klasifikācijas rezultātu ar Open StreetMap datiem.</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē ūdenstilpes (&gt;1 ha) tuvumu, kur 100 punkti atbilst atrašānās ūdenstipē vai tās krastā, 0 punkti &gt;1km attālumā. Ūdenstilpju slānis iegūts kombinējot Zemes seguma klasifikācijas rezultātu ar Open StreetMap datiem.</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē ūdenstilpes (&gt;50 ha) tuvumu, kur 100 punkti atbilst atrašānās ūdenstipē vai tās krastā, 0 punkti &gt;1km attālumā. Ūdenstilpju slānis iegūts kombinējot Zemes seguma klasifikācijas rezultātu ar Open StreetMap datiem.</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē meža (&gt;0,1 ha) tuvumu, kur 100 punkti atbilst atrašānās mežā vai tā malā, 0 punkti &gt;1km attālumā. Mežu slānis iegūts no Zemes seguma klasifikācijas rezultāta.</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē meža (&gt;1 ha) tuvumu, kur 100 punkti atbilst atrašānās mežā vai tā malā, 0 punkti &gt;1km attālumā. Mežu slānis iegūts no Zemes seguma klasifikācijas rezultāta.</t>
-  </si>
-  <si>
-    <t>10501.tif</t>
-  </si>
-  <si>
-    <t>Zālāji (&gt;0,1 ha)</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē zālāju (&gt;0,1 ha) tuvumu, kur 100 punkti atbilst atrašānās zālājā vai tā malā, 0 punkti &gt;1km attālumā. Zālāju slānis iegūts no Zemes seguma klasifikācijas rezultāta, kombinējot ar Lauku atbalsta dienesta datiem.</t>
-  </si>
-  <si>
-    <t>10502.tif</t>
-  </si>
-  <si>
-    <t>Zālāji (&gt;1 ha)</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē zālāju (&gt;1 ha) tuvumu, kur 100 punkti atbilst atrašānās zālājā vai tā malā, 0 punkti &gt;1km attālumā. Zālāju slānis iegūts no Zemes seguma klasifikācijas rezultāta, kombinējot ar Lauku atbalsta dienesta datiem.</t>
-  </si>
-  <si>
-    <t>10503.tif</t>
-  </si>
-  <si>
-    <t>Zālāji (bioloģiski vērtīgie)</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē bioloģiski vērtīgo zālāju tuvumu, kur 100 punkti atbilst atrašānās zālājā vai tā malā, 0 punkti &gt;1km attālumā. Bioloģiski vērtīgo zālāju slānis iegūts no Lauku atbalsta dienesta datiem.</t>
-  </si>
-  <si>
-    <t>Lauksaimniecība (&gt;0,1 ha)</t>
-  </si>
-  <si>
-    <t>Lauksaimniecība (1 ha)</t>
-  </si>
-  <si>
-    <t>Lauksaimniecība (bioloģiskā)</t>
-  </si>
-  <si>
-    <t>Lauksaimniecība (konvencionālā)</t>
-  </si>
-  <si>
-    <t>10601.tif</t>
-  </si>
-  <si>
-    <t>10602.tif</t>
-  </si>
-  <si>
-    <t>10603.tif</t>
-  </si>
-  <si>
-    <t>10604.tif</t>
-  </si>
-  <si>
-    <t>10803.tif</t>
-  </si>
-  <si>
-    <t>Ēkas</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē ēku tuvumu, kur 100 punkti atbilst atrašānās ēkā vai pie tās, 0 punkti &gt;1km attālumā. Ēku slānis iegūts no OpenStreetMap datiem.</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē konvencionāli apsaimniekoto lauksaimniecības zemju tuvumu, kur 100 punkti atbilst atrašānās laukā vai tā malā, 0 punkti &gt;1km attālumā. Lauksaimniecības zemju slānis iegūts no Zemes seguma klasifikācijas rezultāta, kombinējot ar Lauku atbalsta dienesta datiem.</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē bioloģiski apsaimniekoto lauksaimniecības zemju tuvumu, kur 100 punkti atbilst atrašānās laukā vai tā malā, 0 punkti &gt;1km attālumā. Lauksaimniecības zemju slānis iegūts no Zemes seguma klasifikācijas rezultāta, kombinējot ar Lauku atbalsta dienesta datiem.</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē lauksaimniecības zemju (&gt;1 ha) tuvumu, kur 100 punkti atbilst atrašānās laukā vai tā malā, 0 punkti &gt;1km attālumā. Lauksaimniecības zemju slānis iegūts no Zemes seguma klasifikācijas rezultāta, kombinējot ar Lauku atbalsta dienesta datiem.</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē lauksaimniecības zemju (&gt;0,1 ha) tuvumu, kur 100 punkti atbilst atrašānās laukā vai tā malā, 0 punkti &gt;1km attālumā. Lauksaimniecības zemju slānis iegūts no Zemes seguma klasifikācijas rezultāta, kombinējot ar Lauku atbalsta dienesta datiem.</t>
-  </si>
-  <si>
-    <t>10805.tif</t>
-  </si>
-  <si>
-    <t>Industriāli objekti</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē industriālu objektu tuvumu, kur 100 punkti atbilst atrašānās objektā vai pie tā, 0 punkti &gt;1km attālumā. Industriālo objektu slānis iegūts no OpenStreetMap datiem.</t>
-  </si>
-  <si>
-    <t>10901.tif</t>
-  </si>
-  <si>
-    <t>10902.tif</t>
-  </si>
-  <si>
-    <t>10904.tif</t>
-  </si>
-  <si>
-    <t>Ceļi (visi)</t>
-  </si>
-  <si>
-    <t>Ceļi (galvenie)</t>
-  </si>
-  <si>
-    <t>Dzelzceļš</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē ar auto izbraucamo ceļu tuvumu, kur 100 punkti atbilst atrašānās uz ceļa vai pie tā, 0 punkti &gt;1km attālumā. Ceļu slānis iegūts no OpenStreetMap datiem.</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē galveno ceļu tuvumu, kur 100 punkti atbilst atrašānās uz ceļa vai pie tā, 0 punkti &gt;1km attālumā. Ceļu slānis iegūts no OpenStreetMap datiem.</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē dzelzceļa tuvumu, kur 100 punkti atbilst atrašānās uz dzelzceļa vai pie tā, 0 punkti &gt;1km attālumā. Dzelzceļa slānis iegūts no OpenStreetMap datiem.</t>
-  </si>
-  <si>
-    <t>11001.tif</t>
-  </si>
-  <si>
-    <t>11002.tif</t>
-  </si>
-  <si>
-    <t>11003.tif</t>
-  </si>
-  <si>
-    <t>Tūrisma objekti</t>
-  </si>
-  <si>
-    <t>Kapsētas</t>
-  </si>
-  <si>
-    <t>Militārie objekti</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē tūrisma objektu tuvumu, kur 100 punkti atbilst atrašānās tūrisma objektā, 0 punkti &gt;1km attālumā. Tūrisma objektu slānis iegūts no OpenStreetMap datiem.</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē militāro objektu tuvumu, kur 100 punkti atbilst atrašānās objektā vai pie tā, 0 punkti &gt;1km attālumā. Militāro objektu slānis iegūts no OpenStreetMap datiem.</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē kapsētu tuvumu, kur 100 punkti atbilst atrašānās kapsētā vai pie tās, 0 punkti &gt;1km attālumā. Kapsētu slānis iegūts no OpenStreetMap datiem.</t>
-  </si>
-  <si>
-    <t>11106.tif</t>
-  </si>
-  <si>
-    <t>11107.tif</t>
-  </si>
-  <si>
-    <t>11108.tif</t>
-  </si>
-  <si>
-    <t>11109.tif</t>
-  </si>
-  <si>
-    <t>Zaļums (pastāvīgs)</t>
-  </si>
-  <si>
-    <t>Zaļums (2020)</t>
-  </si>
-  <si>
-    <t>Zaļuma pieaugums</t>
-  </si>
-  <si>
-    <t>Zaļuma samazinājums</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē ainavas procentuālo segumu ar veģetāciju, kur 100 punkti atbilst 100% veģetācijas segumam 300 m diametrā, bet 0 punkti - 0%. Pastāvīgā zaļuma novērtējumam izmantoti Sentinel-2 satelītdati 2016.-2019. gadam, NDVI slieksnis 0,5.</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē ainavas procentuālo veģetācijas segumu 2019. gadā, kur 100 punkti atbilst 100% veģetācijas segumam 300 m diametrā, bet 0 punkti - 0%. Pastāvīgā zaļuma novērtējumam izmantoti Sentinel-2 satelītdati 2019. gadam, NDVI slieksnis 0,5.</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē ainavas procentuālo īpatsvaru ar novērotu zaļuma pieaugumu 2016.-2019. gadā, kur 100 punkti atbilst 100% zaļuma pieaugumam 300 m diametrā, bet 0 punkti - 0%. Zaļuma pieauguma novērtējumam izmantoti Sentinel-2 satelītdati 2016.-2019. gadam, NDVI slieksnis 0,5, skatīta tendence.</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē ainavas procentuālo īpatsvaru ar novērotu zaļuma samazinājumu 2016.-2019. gadā, kur 100 punkti atbilst 100% zaļuma samazinājumam 300 m diametrā, bet 0 punkti - 0%. Zaļuma samazinājuma novērtējumam izmantoti Sentinel-2 satelītdati 2016.-2019. gadam, NDVI slieksnis 0,5, skatīta tendence.</t>
-  </si>
-  <si>
-    <t>11201.tif</t>
-  </si>
-  <si>
-    <t>11202.tif</t>
-  </si>
-  <si>
-    <t>11203.tif</t>
-  </si>
-  <si>
-    <t>Ainavas atvērtums</t>
-  </si>
-  <si>
-    <t>Lokālie pauguri</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē ainavas atvērtumu 300 m radiusā, skatoties no 1,8 m augstuma, kur 100 punkti atbilst pilnīgi atvērtai jeb pārskatāmai ainavai, bet 0 punkti - slēgtai. Datu slāņa izveidei izmantots digitālais virsmas un reljefa modelis.</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē paugurus lokālā reljefā, kur par referenci ņemts vidējais reljefs 300 m radiusā. 100 punkti atbilst pauguram, kas par 10 un vairām metriem paceļas virs vidējā ainavas augstuma, 90 punkti - 9 m, bet 0 punkti vidējam lokālā reljefa augstumam vai zemākam.</t>
-  </si>
-  <si>
-    <t>Datu slānis reprezentē ieplakas lokālā reljefā, kur par referenci ņemts vidējais reljefs 300 m radiusā. 100 punkti atbilst ieplakai, kas par 10 un vairām metriem iegrimst zem vidējā ainavas augstuma, 90 punkti - 9 m, bet 0 punkti vidējam lokālā reljefa augstumam vai augstākam.</t>
-  </si>
-  <si>
-    <t>Lokālās ieplakas</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Layer</t>
-  </si>
-  <si>
-    <t>Comment</t>
+    <t>10701.tif</t>
+  </si>
+  <si>
+    <t>10702.tif</t>
+  </si>
+  <si>
+    <t>10801.tif</t>
+  </si>
+  <si>
+    <t>10802.tif</t>
+  </si>
+  <si>
+    <t>10903.tif</t>
+  </si>
+  <si>
+    <t>11101.tif</t>
+  </si>
+  <si>
+    <t>11102.tif</t>
+  </si>
+  <si>
+    <t>11103.tif</t>
+  </si>
+  <si>
+    <t>Lauksaimniecība</t>
+  </si>
+  <si>
+    <t>Tuvums līdz Cēsīm</t>
+  </si>
+  <si>
+    <t>Tuvums līdz novada centram</t>
+  </si>
+  <si>
+    <t>Tuvums līdz sekundāram centram</t>
   </si>
 </sst>
 </file>
@@ -693,11 +621,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6EB2E9C-8014-4123-9692-528EC0826580}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,370 +637,282 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C33">
-    <sortCondition ref="A1:A33"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C25">
+    <sortCondition ref="A1:A25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>